<commit_message>
new sentitivity and calculus
</commit_message>
<xml_diff>
--- a/data/results/daily_model/daily_model_results_(-0.1, 0.1, 0.1).xlsx
+++ b/data/results/daily_model/daily_model_results_(-0.1, 0.1, 0.1).xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,6 +445,31 @@
           <t>Accuracy (%)</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Market threshold</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Market min</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Market max</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Recall</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Precision</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -453,7 +478,22 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>32.88508557457212</v>
+        <v>32.94621026894865</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.05450546436368681</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-15.55441</v>
+      </c>
+      <c r="E2" t="n">
+        <v>15.06418</v>
+      </c>
+      <c r="F2" t="n">
+        <v>11.11111111111111</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1.098901098901099</v>
       </c>
     </row>
     <row r="3">
@@ -463,7 +503,22 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>30.07334963325183</v>
+        <v>27.13936430317848</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.009583939973006913</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-19.35264</v>
+      </c>
+      <c r="E3" t="n">
+        <v>13.70093</v>
+      </c>
+      <c r="F3" t="n">
+        <v>14.20911528150134</v>
+      </c>
+      <c r="G3" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="4">
@@ -473,7 +528,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>52.20048899755502</v>
+        <v>51.83374083129584</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.04158117063764853</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-18.75314</v>
+      </c>
+      <c r="E4" t="n">
+        <v>23.33066</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -483,7 +553,22 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>43.64303178484107</v>
+        <v>41.80929095354523</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.02983403801513819</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-12.78028</v>
+      </c>
+      <c r="E5" t="n">
+        <v>12.42348</v>
+      </c>
+      <c r="F5" t="n">
+        <v>14.54545454545454</v>
+      </c>
+      <c r="G5" t="n">
+        <v>6.083650190114068</v>
       </c>
     </row>
     <row r="6">
@@ -493,7 +578,22 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>43.33740831295844</v>
+        <v>43.94865525672372</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.08368817696170747</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-16.47904</v>
+      </c>
+      <c r="E6" t="n">
+        <v>14.94325</v>
+      </c>
+      <c r="F6" t="n">
+        <v>50</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.3603603603603603</v>
       </c>
     </row>
   </sheetData>
@@ -558,10 +658,10 @@
         <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="D3" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
@@ -571,13 +671,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="D4" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -623,13 +723,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="C2" t="n">
-        <v>208</v>
+        <v>110</v>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3">
@@ -639,13 +739,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="C3" t="n">
-        <v>478</v>
+        <v>223</v>
       </c>
       <c r="D3" t="n">
-        <v>5</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4">
@@ -655,13 +755,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>13</v>
+        <v>196</v>
       </c>
       <c r="C4" t="n">
-        <v>658</v>
+        <v>319</v>
       </c>
       <c r="D4" t="n">
-        <v>12</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -723,13 +823,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C3" t="n">
-        <v>844</v>
+        <v>830</v>
       </c>
       <c r="D3" t="n">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4">
@@ -739,13 +839,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C4" t="n">
-        <v>632</v>
+        <v>619</v>
       </c>
       <c r="D4" t="n">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -791,13 +891,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C2" t="n">
-        <v>254</v>
+        <v>232</v>
       </c>
       <c r="D2" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">
@@ -807,13 +907,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="C3" t="n">
-        <v>700</v>
+        <v>621</v>
       </c>
       <c r="D3" t="n">
-        <v>8</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4">
@@ -823,13 +923,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="C4" t="n">
-        <v>573</v>
+        <v>505</v>
       </c>
       <c r="D4" t="n">
-        <v>11</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -875,13 +975,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>545</v>
+        <v>552</v>
       </c>
       <c r="D2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -891,13 +991,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>701</v>
+        <v>716</v>
       </c>
       <c r="D3" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -907,13 +1007,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="D4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>